<commit_message>
Changed the description for the ice blocks
</commit_message>
<xml_diff>
--- a/Project Documents/Ice Block.xlsx
+++ b/Project Documents/Ice Block.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00198403\Documents\Push-Penguin-3D\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00198403\Desktop\GIT\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Characters</t>
   </si>
@@ -63,18 +63,9 @@
     <t>Describe Role in game</t>
   </si>
   <si>
-    <t>Text description of role in game</t>
-  </si>
-  <si>
     <t>Internal Functionality</t>
   </si>
   <si>
-    <t>Eg Turn Left</t>
-  </si>
-  <si>
-    <t>Eg Push</t>
-  </si>
-  <si>
     <t>External Outgoing</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>Parameters</t>
   </si>
   <si>
-    <t>ShouldTurnLeft</t>
-  </si>
-  <si>
     <t xml:space="preserve">Return </t>
   </si>
   <si>
@@ -118,14 +106,85 @@
   </si>
   <si>
     <t>Ice Blocks</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>Moving the IceBlock</t>
+  </si>
+  <si>
+    <t>Collision</t>
+  </si>
+  <si>
+    <t>Detecting collisions</t>
+  </si>
+  <si>
+    <t>CheckForAction</t>
+  </si>
+  <si>
+    <t>Checks if the IceBlock should crush an Enemie, Stops, Explodes or continue moving</t>
+  </si>
+  <si>
+    <t>CheckForMovement</t>
+  </si>
+  <si>
+    <t>Checks if the world allows us to move</t>
+  </si>
+  <si>
+    <t>GetPushed</t>
+  </si>
+  <si>
+    <t>If the IceBlock gets a Push, this funktion should be called</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>ChangeStatus</t>
+  </si>
+  <si>
+    <t>This function should set the internal status of the iceblock (standing still, moving…)</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>IceBlock.Status</t>
+  </si>
+  <si>
+    <t>Distance / Integer</t>
+  </si>
+  <si>
+    <t>The IceBlock can be used to cursh a enemie, change the setup of the world or can get destroyed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,8 +212,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +533,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -522,12 +583,12 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -542,7 +603,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -583,95 +644,152 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="76" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>